<commit_message>
fix : problème de  création de statistique et  type variable optimizer
</commit_message>
<xml_diff>
--- a/batch_experiments/2026_02_07/T7200/V5_03_C/scores_summary.xlsx
+++ b/batch_experiments/2026_02_07/T7200/V5_03_C/scores_summary.xlsx
@@ -918,7 +918,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>32,565,840</t>
+          <t>32,565,840.0</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>35,828,440</t>
+          <t>35,828,440.0</t>
         </is>
       </c>
     </row>

</xml_diff>